<commit_message>
add colum with numbers
</commit_message>
<xml_diff>
--- a/Test Spreadsheet.xlsx
+++ b/Test Spreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>person 1</t>
+  </si>
+  <si>
+    <t>person 2</t>
+  </si>
+  <si>
+    <t>person 3</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>salesman</t>
+  </si>
+  <si>
+    <t>accountant</t>
+  </si>
+  <si>
+    <t>programmer</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +81,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +170,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +378,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test for a branch b1
</commit_message>
<xml_diff>
--- a/Test Spreadsheet.xlsx
+++ b/Test Spreadsheet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -44,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,13 +52,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,54 +395,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <f>C3*2</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
another commit for branch b1
</commit_message>
<xml_diff>
--- a/Test Spreadsheet.xlsx
+++ b/Test Spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>person 1</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>programmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person 4 </t>
+  </si>
+  <si>
+    <t>QA</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,8 +451,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <f>C3*2</f>
-        <v>6</v>
+        <f>C3*2*2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition in master for merge testing
</commit_message>
<xml_diff>
--- a/Test Spreadsheet.xlsx
+++ b/Test Spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>person 1</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>programmer</t>
+  </si>
+  <si>
+    <t>back to master</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +431,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>